<commit_message>
update and some bugs
</commit_message>
<xml_diff>
--- a/btpy/src/btpy/res/lastname_data.xlsx
+++ b/btpy/src/btpy/res/lastname_data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="1238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="1400">
   <si>
     <t>russian</t>
   </si>
@@ -2624,6 +2624,288 @@
     <t>Yakano</t>
   </si>
   <si>
+    <t>Toriyama</t>
+  </si>
+  <si>
+    <t>Hayashi</t>
+  </si>
+  <si>
+    <t>Hatake</t>
+  </si>
+  <si>
+    <t>Osaka</t>
+  </si>
+  <si>
+    <t>Tee</t>
+  </si>
+  <si>
+    <t>Yamazaki</t>
+  </si>
+  <si>
+    <t>Misaki</t>
+  </si>
+  <si>
+    <t>Hokusai</t>
+  </si>
+  <si>
+    <t>Kusama</t>
+  </si>
+  <si>
+    <t>Ogata</t>
+  </si>
+  <si>
+    <t>Tendo</t>
+  </si>
+  <si>
+    <t>Sugimoto</t>
+  </si>
+  <si>
+    <t>Nara</t>
+  </si>
+  <si>
+    <t>Shiraga</t>
+  </si>
+  <si>
+    <t>Ohtake</t>
+  </si>
+  <si>
+    <t>Kendo</t>
+  </si>
+  <si>
+    <t>Haruno</t>
+  </si>
+  <si>
+    <t>Yashida</t>
+  </si>
+  <si>
+    <t>Kishibe</t>
+  </si>
+  <si>
+    <t>Aruga</t>
+  </si>
+  <si>
+    <t>Arima</t>
+  </si>
+  <si>
+    <t>Hosogaya</t>
+  </si>
+  <si>
+    <t>Takeaki</t>
+  </si>
+  <si>
+    <t>Jojima</t>
+  </si>
+  <si>
+    <t>Yoshika</t>
+  </si>
+  <si>
+    <t>Ijichi</t>
+  </si>
+  <si>
+    <t>Sukenori</t>
+  </si>
+  <si>
+    <t>Kakuta</t>
+  </si>
+  <si>
+    <t>Sadakichi</t>
+  </si>
+  <si>
+    <t>Tamosaburo</t>
+  </si>
+  <si>
+    <t>Kawamura</t>
+  </si>
+  <si>
+    <t>Koga</t>
+  </si>
+  <si>
+    <t>Kurita</t>
+  </si>
+  <si>
+    <t>Kusaka</t>
+  </si>
+  <si>
+    <t>Mikawa</t>
+  </si>
+  <si>
+    <t>Nagumo</t>
+  </si>
+  <si>
+    <t>Nishimura</t>
+  </si>
+  <si>
+    <t>Nobutake</t>
+  </si>
+  <si>
+    <t>Onishi</t>
+  </si>
+  <si>
+    <t>Ota</t>
+  </si>
+  <si>
+    <t>Ozawa</t>
+  </si>
+  <si>
+    <t>Takagi</t>
+  </si>
+  <si>
+    <t>Toyoda</t>
+  </si>
+  <si>
+    <t>Heihachiro</t>
+  </si>
+  <si>
+    <t>Gonbee</t>
+  </si>
+  <si>
+    <t>Yonai</t>
+  </si>
+  <si>
+    <t>Cho</t>
+  </si>
+  <si>
+    <t>Bada</t>
+  </si>
+  <si>
+    <t>Doihara</t>
+  </si>
+  <si>
+    <t>Imamura</t>
+  </si>
+  <si>
+    <t>Itagaki</t>
+  </si>
+  <si>
+    <t>Taro</t>
+  </si>
+  <si>
+    <t>Kenichi</t>
+  </si>
+  <si>
+    <t>Gentaro</t>
+  </si>
+  <si>
+    <t>Koiso</t>
+  </si>
+  <si>
+    <t>Katsuyoshi</t>
+  </si>
+  <si>
+    <t>Kiyotaka</t>
+  </si>
+  <si>
+    <t>Tamemoto</t>
+  </si>
+  <si>
+    <t>No Noriyori</t>
+  </si>
+  <si>
+    <t>Muto</t>
+  </si>
+  <si>
+    <t>Nishio</t>
+  </si>
+  <si>
+    <t>Nishida</t>
+  </si>
+  <si>
+    <t>Sa-ik</t>
+  </si>
+  <si>
+    <t>Asaka</t>
+  </si>
+  <si>
+    <t>Goro</t>
+  </si>
+  <si>
+    <t>Aritomo</t>
+  </si>
+  <si>
+    <t>Motoharu</t>
+  </si>
+  <si>
+    <t>Hanzo</t>
+  </si>
+  <si>
+    <t>Yamashita</t>
+  </si>
+  <si>
+    <t>Yasuku</t>
+  </si>
+  <si>
+    <t>Ikari</t>
+  </si>
+  <si>
+    <t>Yagami</t>
+  </si>
+  <si>
+    <t>Kusanagi</t>
+  </si>
+  <si>
+    <t>Kujo</t>
+  </si>
+  <si>
+    <t>Kamodo</t>
+  </si>
+  <si>
+    <t>Shinazugawa</t>
+  </si>
+  <si>
+    <t>Kocho</t>
+  </si>
+  <si>
+    <t>Agatsuma</t>
+  </si>
+  <si>
+    <t>Tomioka</t>
+  </si>
+  <si>
+    <t>Tsuyuri</t>
+  </si>
+  <si>
+    <t>Kibutsuji</t>
+  </si>
+  <si>
+    <t>Iguro</t>
+  </si>
+  <si>
+    <t>Uzui</t>
+  </si>
+  <si>
+    <t>Urokodaki</t>
+  </si>
+  <si>
+    <t>Kanzaki</t>
+  </si>
+  <si>
+    <t>Kamado</t>
+  </si>
+  <si>
+    <t>Himejima</t>
+  </si>
+  <si>
+    <t>Aburame</t>
+  </si>
+  <si>
+    <t>Yamanaka</t>
+  </si>
+  <si>
+    <t>Kanemaru</t>
+  </si>
+  <si>
+    <t>Magonojo</t>
+  </si>
+  <si>
+    <t>Munisai</t>
+  </si>
+  <si>
+    <t>Gozen</t>
+  </si>
+  <si>
+    <t>Kiniyoshi</t>
+  </si>
+  <si>
     <t>polinesian</t>
   </si>
   <si>
@@ -3741,6 +4023,210 @@
   </si>
   <si>
     <t>Rosati</t>
+  </si>
+  <si>
+    <t>hebrew</t>
+  </si>
+  <si>
+    <t>Cohen</t>
+  </si>
+  <si>
+    <t>Levy</t>
+  </si>
+  <si>
+    <t>Mizrahi</t>
+  </si>
+  <si>
+    <t>Peretz</t>
+  </si>
+  <si>
+    <t>Bitton</t>
+  </si>
+  <si>
+    <t>Dahan</t>
+  </si>
+  <si>
+    <t>Agbaria</t>
+  </si>
+  <si>
+    <t>Avraham</t>
+  </si>
+  <si>
+    <t>Katz</t>
+  </si>
+  <si>
+    <t>Yosef</t>
+  </si>
+  <si>
+    <t>Omer</t>
+  </si>
+  <si>
+    <t>Mhamid</t>
+  </si>
+  <si>
+    <t>Dohan</t>
+  </si>
+  <si>
+    <t>Abramov</t>
+  </si>
+  <si>
+    <t>Azoulai</t>
+  </si>
+  <si>
+    <t>Malka</t>
+  </si>
+  <si>
+    <t>Hadad</t>
+  </si>
+  <si>
+    <t>Amar</t>
+  </si>
+  <si>
+    <t>Gaddai</t>
+  </si>
+  <si>
+    <t>Edri</t>
+  </si>
+  <si>
+    <t>Tal</t>
+  </si>
+  <si>
+    <t>Shapira</t>
+  </si>
+  <si>
+    <t>Hazan</t>
+  </si>
+  <si>
+    <t>Moshe</t>
+  </si>
+  <si>
+    <t>Ohana</t>
+  </si>
+  <si>
+    <t>Segal</t>
+  </si>
+  <si>
+    <t>Golan</t>
+  </si>
+  <si>
+    <t>Yitzhak</t>
+  </si>
+  <si>
+    <t>Bar</t>
+  </si>
+  <si>
+    <t>Yaakov</t>
+  </si>
+  <si>
+    <t>Shalom</t>
+  </si>
+  <si>
+    <t>Mor</t>
+  </si>
+  <si>
+    <t>Dayan</t>
+  </si>
+  <si>
+    <t>Eliyahu</t>
+  </si>
+  <si>
+    <t>Elbaz</t>
+  </si>
+  <si>
+    <t>Lavi</t>
+  </si>
+  <si>
+    <t>Suissa</t>
+  </si>
+  <si>
+    <t>Shemesh</t>
+  </si>
+  <si>
+    <t>Stern</t>
+  </si>
+  <si>
+    <t>Nachum</t>
+  </si>
+  <si>
+    <t>Alon</t>
+  </si>
+  <si>
+    <t>Rosenberg</t>
+  </si>
+  <si>
+    <t>Sharabi</t>
+  </si>
+  <si>
+    <t>Sasson</t>
+  </si>
+  <si>
+    <t>Bachar</t>
+  </si>
+  <si>
+    <t>Shahar</t>
+  </si>
+  <si>
+    <t>Maimon</t>
+  </si>
+  <si>
+    <t>Ovadia</t>
+  </si>
+  <si>
+    <t>Ben Hemo</t>
+  </si>
+  <si>
+    <t>Vaknin</t>
+  </si>
+  <si>
+    <t>Assouline</t>
+  </si>
+  <si>
+    <t>Meir</t>
+  </si>
+  <si>
+    <t>Amsalem</t>
+  </si>
+  <si>
+    <t>Baruch</t>
+  </si>
+  <si>
+    <t>Rubin</t>
+  </si>
+  <si>
+    <t>Harel</t>
+  </si>
+  <si>
+    <t>Ezra</t>
+  </si>
+  <si>
+    <t>Sabag</t>
+  </si>
+  <si>
+    <t>Yifrah</t>
+  </si>
+  <si>
+    <t>Kadosh</t>
+  </si>
+  <si>
+    <t>Halimi</t>
+  </si>
+  <si>
+    <t>Azulay</t>
+  </si>
+  <si>
+    <t>Gal</t>
+  </si>
+  <si>
+    <t>Nissim</t>
+  </si>
+  <si>
+    <t>Zaken</t>
+  </si>
+  <si>
+    <t>Menashe</t>
+  </si>
+  <si>
+    <t>Abraham</t>
   </si>
 </sst>
 </file>
@@ -4409,7 +4895,14 @@
     <cellStyle name="40% - Énfasis6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Énfasis6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -4685,13 +5178,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:EW16"/>
+  <dimension ref="A2:FS17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DJ4" workbookViewId="0">
-      <selection activeCell="DW9" sqref="DW9"/>
+    <sheetView tabSelected="1" topLeftCell="FI7" workbookViewId="0">
+      <selection activeCell="FS13" sqref="FS13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.7777777777778" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="16384" width="11.7777777777778" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:70">
       <c r="A2" t="s">
@@ -7100,7 +7596,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="13" spans="1:81">
+    <row r="13" spans="1:175">
       <c r="A13" t="s">
         <v>784</v>
       </c>
@@ -7343,1185 +7839,1688 @@
       </c>
       <c r="CC13" t="s">
         <v>864</v>
+      </c>
+      <c r="CD13" t="s">
+        <v>865</v>
+      </c>
+      <c r="CE13" t="s">
+        <v>866</v>
+      </c>
+      <c r="CF13" t="s">
+        <v>867</v>
+      </c>
+      <c r="CG13" t="s">
+        <v>868</v>
+      </c>
+      <c r="CH13" t="s">
+        <v>869</v>
+      </c>
+      <c r="CI13" t="s">
+        <v>870</v>
+      </c>
+      <c r="CJ13" t="s">
+        <v>871</v>
+      </c>
+      <c r="CK13" t="s">
+        <v>872</v>
+      </c>
+      <c r="CL13" t="s">
+        <v>873</v>
+      </c>
+      <c r="CM13" t="s">
+        <v>874</v>
+      </c>
+      <c r="CN13" t="s">
+        <v>875</v>
+      </c>
+      <c r="CO13" t="s">
+        <v>876</v>
+      </c>
+      <c r="CP13" t="s">
+        <v>877</v>
+      </c>
+      <c r="CQ13" t="s">
+        <v>878</v>
+      </c>
+      <c r="CR13" t="s">
+        <v>879</v>
+      </c>
+      <c r="CS13" t="s">
+        <v>880</v>
+      </c>
+      <c r="CT13" t="s">
+        <v>881</v>
+      </c>
+      <c r="CU13" t="s">
+        <v>882</v>
+      </c>
+      <c r="CV13" t="s">
+        <v>883</v>
+      </c>
+      <c r="CW13" t="s">
+        <v>884</v>
+      </c>
+      <c r="CX13" t="s">
+        <v>885</v>
+      </c>
+      <c r="CY13" t="s">
+        <v>886</v>
+      </c>
+      <c r="CZ13" t="s">
+        <v>887</v>
+      </c>
+      <c r="DA13" t="s">
+        <v>888</v>
+      </c>
+      <c r="DB13" t="s">
+        <v>889</v>
+      </c>
+      <c r="DC13" t="s">
+        <v>890</v>
+      </c>
+      <c r="DD13" t="s">
+        <v>891</v>
+      </c>
+      <c r="DE13" t="s">
+        <v>892</v>
+      </c>
+      <c r="DF13" t="s">
+        <v>893</v>
+      </c>
+      <c r="DG13" t="s">
+        <v>894</v>
+      </c>
+      <c r="DH13" t="s">
+        <v>895</v>
+      </c>
+      <c r="DI13" t="s">
+        <v>896</v>
+      </c>
+      <c r="DJ13" t="s">
+        <v>897</v>
+      </c>
+      <c r="DK13" t="s">
+        <v>898</v>
+      </c>
+      <c r="DL13" t="s">
+        <v>899</v>
+      </c>
+      <c r="DM13" t="s">
+        <v>900</v>
+      </c>
+      <c r="DN13" t="s">
+        <v>901</v>
+      </c>
+      <c r="DO13" t="s">
+        <v>902</v>
+      </c>
+      <c r="DP13" t="s">
+        <v>903</v>
+      </c>
+      <c r="DQ13" t="s">
+        <v>904</v>
+      </c>
+      <c r="DR13" t="s">
+        <v>905</v>
+      </c>
+      <c r="DS13" t="s">
+        <v>906</v>
+      </c>
+      <c r="DT13" t="s">
+        <v>907</v>
+      </c>
+      <c r="DU13" t="s">
+        <v>908</v>
+      </c>
+      <c r="DV13" t="s">
+        <v>909</v>
+      </c>
+      <c r="DW13" t="s">
+        <v>910</v>
+      </c>
+      <c r="DX13" t="s">
+        <v>911</v>
+      </c>
+      <c r="DY13" t="s">
+        <v>912</v>
+      </c>
+      <c r="DZ13" t="s">
+        <v>913</v>
+      </c>
+      <c r="EA13" t="s">
+        <v>914</v>
+      </c>
+      <c r="EB13" t="s">
+        <v>915</v>
+      </c>
+      <c r="EC13" t="s">
+        <v>916</v>
+      </c>
+      <c r="ED13" t="s">
+        <v>917</v>
+      </c>
+      <c r="EE13" t="s">
+        <v>918</v>
+      </c>
+      <c r="EF13" t="s">
+        <v>919</v>
+      </c>
+      <c r="EG13" t="s">
+        <v>920</v>
+      </c>
+      <c r="EH13" t="s">
+        <v>921</v>
+      </c>
+      <c r="EI13" t="s">
+        <v>922</v>
+      </c>
+      <c r="EJ13" t="s">
+        <v>923</v>
+      </c>
+      <c r="EK13" t="s">
+        <v>924</v>
+      </c>
+      <c r="EL13" t="s">
+        <v>925</v>
+      </c>
+      <c r="EM13" t="s">
+        <v>926</v>
+      </c>
+      <c r="EN13" t="s">
+        <v>927</v>
+      </c>
+      <c r="EO13" t="s">
+        <v>928</v>
+      </c>
+      <c r="EP13" t="s">
+        <v>929</v>
+      </c>
+      <c r="EQ13" t="s">
+        <v>930</v>
+      </c>
+      <c r="ER13" t="s">
+        <v>931</v>
+      </c>
+      <c r="ES13" t="s">
+        <v>932</v>
+      </c>
+      <c r="ET13" t="s">
+        <v>933</v>
+      </c>
+      <c r="EU13" t="s">
+        <v>934</v>
+      </c>
+      <c r="EV13" t="s">
+        <v>935</v>
+      </c>
+      <c r="EW13" t="s">
+        <v>936</v>
+      </c>
+      <c r="EX13" t="s">
+        <v>937</v>
+      </c>
+      <c r="EY13" t="s">
+        <v>938</v>
+      </c>
+      <c r="EZ13" t="s">
+        <v>939</v>
+      </c>
+      <c r="FA13" t="s">
+        <v>940</v>
+      </c>
+      <c r="FB13" t="s">
+        <v>941</v>
+      </c>
+      <c r="FC13" t="s">
+        <v>942</v>
+      </c>
+      <c r="FD13" t="s">
+        <v>943</v>
+      </c>
+      <c r="FE13" t="s">
+        <v>944</v>
+      </c>
+      <c r="FF13" t="s">
+        <v>945</v>
+      </c>
+      <c r="FG13" t="s">
+        <v>946</v>
+      </c>
+      <c r="FH13" t="s">
+        <v>947</v>
+      </c>
+      <c r="FI13" t="s">
+        <v>948</v>
+      </c>
+      <c r="FJ13" t="s">
+        <v>949</v>
+      </c>
+      <c r="FK13" t="s">
+        <v>950</v>
+      </c>
+      <c r="FL13" t="s">
+        <v>951</v>
+      </c>
+      <c r="FM13" t="s">
+        <v>952</v>
+      </c>
+      <c r="FN13" t="s">
+        <v>953</v>
+      </c>
+      <c r="FO13" t="s">
+        <v>954</v>
+      </c>
+      <c r="FP13" t="s">
+        <v>955</v>
+      </c>
+      <c r="FQ13" t="s">
+        <v>956</v>
+      </c>
+      <c r="FR13" t="s">
+        <v>957</v>
+      </c>
+      <c r="FS13" t="s">
+        <v>958</v>
       </c>
     </row>
     <row r="14" spans="1:84">
       <c r="A14" t="s">
-        <v>865</v>
+        <v>959</v>
       </c>
       <c r="B14" t="s">
-        <v>866</v>
+        <v>960</v>
       </c>
       <c r="C14" t="s">
-        <v>867</v>
+        <v>961</v>
       </c>
       <c r="D14" t="s">
-        <v>868</v>
+        <v>962</v>
       </c>
       <c r="E14" t="s">
-        <v>869</v>
+        <v>963</v>
       </c>
       <c r="F14" t="s">
-        <v>870</v>
+        <v>964</v>
       </c>
       <c r="G14" t="s">
-        <v>871</v>
+        <v>965</v>
       </c>
       <c r="H14" t="s">
-        <v>872</v>
+        <v>966</v>
       </c>
       <c r="I14" t="s">
-        <v>873</v>
+        <v>967</v>
       </c>
       <c r="J14" t="s">
-        <v>874</v>
+        <v>968</v>
       </c>
       <c r="K14" t="s">
-        <v>875</v>
+        <v>969</v>
       </c>
       <c r="L14" t="s">
-        <v>876</v>
+        <v>970</v>
       </c>
       <c r="M14" t="s">
-        <v>877</v>
+        <v>971</v>
       </c>
       <c r="N14" t="s">
         <v>308</v>
       </c>
       <c r="O14" t="s">
-        <v>878</v>
+        <v>972</v>
       </c>
       <c r="P14" t="s">
-        <v>879</v>
+        <v>973</v>
       </c>
       <c r="Q14" t="s">
-        <v>880</v>
+        <v>974</v>
       </c>
       <c r="R14" t="s">
-        <v>881</v>
+        <v>975</v>
       </c>
       <c r="S14" t="s">
-        <v>882</v>
+        <v>976</v>
       </c>
       <c r="T14" t="s">
-        <v>883</v>
+        <v>977</v>
       </c>
       <c r="U14" t="s">
-        <v>884</v>
+        <v>978</v>
       </c>
       <c r="V14" t="s">
         <v>777</v>
       </c>
       <c r="W14" t="s">
-        <v>885</v>
+        <v>979</v>
       </c>
       <c r="X14" t="s">
-        <v>886</v>
+        <v>980</v>
       </c>
       <c r="Y14" t="s">
         <v>689</v>
       </c>
       <c r="Z14" t="s">
-        <v>887</v>
+        <v>981</v>
       </c>
       <c r="AA14" t="s">
         <v>744</v>
       </c>
       <c r="AB14" t="s">
-        <v>888</v>
+        <v>982</v>
       </c>
       <c r="AC14" t="s">
-        <v>889</v>
+        <v>983</v>
       </c>
       <c r="AD14" t="s">
-        <v>890</v>
+        <v>984</v>
       </c>
       <c r="AE14" t="s">
-        <v>891</v>
+        <v>985</v>
       </c>
       <c r="AF14" t="s">
-        <v>892</v>
+        <v>986</v>
       </c>
       <c r="AG14" t="s">
-        <v>893</v>
+        <v>987</v>
       </c>
       <c r="AH14" t="s">
-        <v>894</v>
+        <v>988</v>
       </c>
       <c r="AI14" t="s">
-        <v>895</v>
+        <v>989</v>
       </c>
       <c r="AJ14" t="s">
-        <v>896</v>
+        <v>990</v>
       </c>
       <c r="AK14" t="s">
-        <v>897</v>
+        <v>991</v>
       </c>
       <c r="AL14" t="s">
         <v>711</v>
       </c>
       <c r="AM14" t="s">
-        <v>898</v>
+        <v>992</v>
       </c>
       <c r="AN14" t="s">
-        <v>899</v>
+        <v>993</v>
       </c>
       <c r="AO14" t="s">
-        <v>900</v>
+        <v>994</v>
       </c>
       <c r="AP14" t="s">
-        <v>901</v>
+        <v>995</v>
       </c>
       <c r="AQ14" t="s">
-        <v>902</v>
+        <v>996</v>
       </c>
       <c r="AR14" t="s">
-        <v>903</v>
+        <v>997</v>
       </c>
       <c r="AS14" t="s">
-        <v>904</v>
+        <v>998</v>
       </c>
       <c r="AT14" t="s">
-        <v>905</v>
+        <v>999</v>
       </c>
       <c r="AU14" t="s">
-        <v>906</v>
+        <v>1000</v>
       </c>
       <c r="AV14" t="s">
-        <v>907</v>
+        <v>1001</v>
       </c>
       <c r="AW14" t="s">
-        <v>908</v>
+        <v>1002</v>
       </c>
       <c r="AX14" t="s">
-        <v>909</v>
+        <v>1003</v>
       </c>
       <c r="AY14" t="s">
-        <v>910</v>
+        <v>1004</v>
       </c>
       <c r="AZ14" t="s">
-        <v>911</v>
+        <v>1005</v>
       </c>
       <c r="BA14" t="s">
-        <v>912</v>
+        <v>1006</v>
       </c>
       <c r="BB14" t="s">
-        <v>913</v>
+        <v>1007</v>
       </c>
       <c r="BC14" t="s">
-        <v>914</v>
+        <v>1008</v>
       </c>
       <c r="BD14" t="s">
-        <v>915</v>
+        <v>1009</v>
       </c>
       <c r="BE14" t="s">
-        <v>916</v>
+        <v>1010</v>
       </c>
       <c r="BF14" t="s">
-        <v>917</v>
+        <v>1011</v>
       </c>
       <c r="BG14" t="s">
-        <v>918</v>
+        <v>1012</v>
       </c>
       <c r="BH14" t="s">
-        <v>919</v>
+        <v>1013</v>
       </c>
       <c r="BI14" t="s">
-        <v>920</v>
+        <v>1014</v>
       </c>
       <c r="BJ14" t="s">
-        <v>921</v>
+        <v>1015</v>
       </c>
       <c r="BK14" t="s">
-        <v>922</v>
+        <v>1016</v>
       </c>
       <c r="BL14" t="s">
-        <v>923</v>
+        <v>1017</v>
       </c>
       <c r="BM14" t="s">
-        <v>924</v>
+        <v>1018</v>
       </c>
       <c r="BN14" t="s">
-        <v>925</v>
+        <v>1019</v>
       </c>
       <c r="BO14" t="s">
-        <v>926</v>
+        <v>1020</v>
       </c>
       <c r="BP14" t="s">
-        <v>927</v>
+        <v>1021</v>
       </c>
       <c r="BQ14" t="s">
         <v>704</v>
       </c>
       <c r="BR14" t="s">
-        <v>928</v>
+        <v>1022</v>
       </c>
       <c r="BS14" t="s">
-        <v>929</v>
+        <v>1023</v>
       </c>
       <c r="BT14" t="s">
         <v>706</v>
       </c>
       <c r="BU14" t="s">
-        <v>930</v>
+        <v>1024</v>
       </c>
       <c r="BV14" t="s">
-        <v>931</v>
+        <v>1025</v>
       </c>
       <c r="BW14" t="s">
-        <v>932</v>
+        <v>1026</v>
       </c>
       <c r="BX14" t="s">
-        <v>933</v>
+        <v>1027</v>
       </c>
       <c r="BY14" t="s">
-        <v>934</v>
+        <v>1028</v>
       </c>
       <c r="BZ14" t="s">
-        <v>935</v>
+        <v>1029</v>
       </c>
       <c r="CA14" t="s">
         <v>694</v>
       </c>
       <c r="CB14" t="s">
-        <v>936</v>
+        <v>1030</v>
       </c>
       <c r="CC14" t="s">
-        <v>937</v>
+        <v>1031</v>
       </c>
       <c r="CD14" t="s">
         <v>701</v>
       </c>
       <c r="CE14" t="s">
-        <v>938</v>
+        <v>1032</v>
       </c>
       <c r="CF14" t="s">
-        <v>939</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="15" spans="1:153">
       <c r="A15" t="s">
-        <v>940</v>
+        <v>1034</v>
       </c>
       <c r="B15" t="s">
-        <v>941</v>
+        <v>1035</v>
       </c>
       <c r="C15" t="s">
-        <v>942</v>
+        <v>1036</v>
       </c>
       <c r="D15" t="s">
-        <v>943</v>
+        <v>1037</v>
       </c>
       <c r="E15" t="s">
-        <v>944</v>
+        <v>1038</v>
       </c>
       <c r="F15" t="s">
-        <v>945</v>
+        <v>1039</v>
       </c>
       <c r="G15" t="s">
-        <v>946</v>
+        <v>1040</v>
       </c>
       <c r="H15" t="s">
-        <v>947</v>
+        <v>1041</v>
       </c>
       <c r="I15" t="s">
-        <v>948</v>
+        <v>1042</v>
       </c>
       <c r="J15" t="s">
-        <v>949</v>
+        <v>1043</v>
       </c>
       <c r="K15" t="s">
-        <v>950</v>
+        <v>1044</v>
       </c>
       <c r="L15" t="s">
-        <v>951</v>
+        <v>1045</v>
       </c>
       <c r="M15" t="s">
-        <v>952</v>
+        <v>1046</v>
       </c>
       <c r="N15" t="s">
-        <v>953</v>
+        <v>1047</v>
       </c>
       <c r="O15" t="s">
-        <v>954</v>
+        <v>1048</v>
       </c>
       <c r="P15" t="s">
-        <v>955</v>
+        <v>1049</v>
       </c>
       <c r="Q15" t="s">
-        <v>956</v>
+        <v>1050</v>
       </c>
       <c r="R15" t="s">
-        <v>957</v>
+        <v>1051</v>
       </c>
       <c r="S15" t="s">
-        <v>958</v>
+        <v>1052</v>
       </c>
       <c r="T15" t="s">
-        <v>959</v>
+        <v>1053</v>
       </c>
       <c r="U15" t="s">
-        <v>960</v>
+        <v>1054</v>
       </c>
       <c r="V15" t="s">
-        <v>961</v>
+        <v>1055</v>
       </c>
       <c r="W15" t="s">
-        <v>962</v>
+        <v>1056</v>
       </c>
       <c r="X15" t="s">
-        <v>963</v>
+        <v>1057</v>
       </c>
       <c r="Y15" t="s">
-        <v>964</v>
+        <v>1058</v>
       </c>
       <c r="Z15" t="s">
-        <v>965</v>
+        <v>1059</v>
       </c>
       <c r="AA15" t="s">
-        <v>966</v>
+        <v>1060</v>
       </c>
       <c r="AB15" t="s">
-        <v>967</v>
+        <v>1061</v>
       </c>
       <c r="AC15" t="s">
-        <v>968</v>
+        <v>1062</v>
       </c>
       <c r="AD15" t="s">
-        <v>969</v>
+        <v>1063</v>
       </c>
       <c r="AE15" t="s">
-        <v>970</v>
+        <v>1064</v>
       </c>
       <c r="AF15" t="s">
-        <v>971</v>
+        <v>1065</v>
       </c>
       <c r="AG15" t="s">
-        <v>972</v>
+        <v>1066</v>
       </c>
       <c r="AH15" t="s">
-        <v>973</v>
+        <v>1067</v>
       </c>
       <c r="AI15" t="s">
-        <v>974</v>
+        <v>1068</v>
       </c>
       <c r="AJ15" t="s">
-        <v>975</v>
+        <v>1069</v>
       </c>
       <c r="AK15" t="s">
-        <v>976</v>
+        <v>1070</v>
       </c>
       <c r="AL15" t="s">
-        <v>977</v>
+        <v>1071</v>
       </c>
       <c r="AM15" t="s">
-        <v>978</v>
+        <v>1072</v>
       </c>
       <c r="AN15" t="s">
-        <v>979</v>
+        <v>1073</v>
       </c>
       <c r="AO15" t="s">
-        <v>980</v>
+        <v>1074</v>
       </c>
       <c r="AP15" t="s">
-        <v>981</v>
+        <v>1075</v>
       </c>
       <c r="AQ15" t="s">
-        <v>982</v>
+        <v>1076</v>
       </c>
       <c r="AR15" t="s">
-        <v>983</v>
+        <v>1077</v>
       </c>
       <c r="AS15" t="s">
         <v>596</v>
       </c>
       <c r="AT15" t="s">
-        <v>984</v>
+        <v>1078</v>
       </c>
       <c r="AU15" t="s">
-        <v>985</v>
+        <v>1079</v>
       </c>
       <c r="AV15" t="s">
-        <v>986</v>
+        <v>1080</v>
       </c>
       <c r="AW15" t="s">
-        <v>987</v>
+        <v>1081</v>
       </c>
       <c r="AX15" t="s">
-        <v>988</v>
+        <v>1082</v>
       </c>
       <c r="AY15" t="s">
-        <v>989</v>
+        <v>1083</v>
       </c>
       <c r="AZ15" t="s">
-        <v>990</v>
+        <v>1084</v>
       </c>
       <c r="BA15" t="s">
-        <v>991</v>
+        <v>1085</v>
       </c>
       <c r="BB15" t="s">
-        <v>992</v>
+        <v>1086</v>
       </c>
       <c r="BC15" t="s">
-        <v>993</v>
+        <v>1087</v>
       </c>
       <c r="BD15" t="s">
-        <v>994</v>
+        <v>1088</v>
       </c>
       <c r="BE15" t="s">
-        <v>995</v>
+        <v>1089</v>
       </c>
       <c r="BF15" t="s">
-        <v>996</v>
+        <v>1090</v>
       </c>
       <c r="BG15" t="s">
-        <v>997</v>
+        <v>1091</v>
       </c>
       <c r="BH15" t="s">
-        <v>998</v>
+        <v>1092</v>
       </c>
       <c r="BI15" t="s">
-        <v>999</v>
+        <v>1093</v>
       </c>
       <c r="BJ15" t="s">
-        <v>1000</v>
+        <v>1094</v>
       </c>
       <c r="BK15" t="s">
-        <v>1001</v>
+        <v>1095</v>
       </c>
       <c r="BL15" t="s">
-        <v>1002</v>
+        <v>1096</v>
       </c>
       <c r="BM15" t="s">
-        <v>1003</v>
+        <v>1097</v>
       </c>
       <c r="BN15" t="s">
-        <v>1004</v>
+        <v>1098</v>
       </c>
       <c r="BO15" t="s">
-        <v>1005</v>
+        <v>1099</v>
       </c>
       <c r="BP15" t="s">
-        <v>1006</v>
+        <v>1100</v>
       </c>
       <c r="BQ15" t="s">
-        <v>1007</v>
+        <v>1101</v>
       </c>
       <c r="BR15" t="s">
-        <v>1008</v>
+        <v>1102</v>
       </c>
       <c r="BS15" t="s">
-        <v>1009</v>
+        <v>1103</v>
       </c>
       <c r="BT15" t="s">
-        <v>1010</v>
+        <v>1104</v>
       </c>
       <c r="BU15" t="s">
-        <v>1011</v>
+        <v>1105</v>
       </c>
       <c r="BV15" t="s">
-        <v>1012</v>
+        <v>1106</v>
       </c>
       <c r="BW15" t="s">
-        <v>1013</v>
+        <v>1107</v>
       </c>
       <c r="BX15" t="s">
-        <v>1014</v>
+        <v>1108</v>
       </c>
       <c r="BY15" t="s">
-        <v>1015</v>
+        <v>1109</v>
       </c>
       <c r="BZ15" t="s">
-        <v>1016</v>
+        <v>1110</v>
       </c>
       <c r="CA15" t="s">
-        <v>1017</v>
+        <v>1111</v>
       </c>
       <c r="CB15" t="s">
-        <v>1018</v>
+        <v>1112</v>
       </c>
       <c r="CC15" t="s">
-        <v>1019</v>
+        <v>1113</v>
       </c>
       <c r="CD15" t="s">
-        <v>1020</v>
+        <v>1114</v>
       </c>
       <c r="CE15" t="s">
-        <v>1021</v>
+        <v>1115</v>
       </c>
       <c r="CF15" t="s">
-        <v>1022</v>
+        <v>1116</v>
       </c>
       <c r="CG15" t="s">
-        <v>1023</v>
+        <v>1117</v>
       </c>
       <c r="CH15" t="s">
-        <v>1024</v>
+        <v>1118</v>
       </c>
       <c r="CI15" t="s">
-        <v>1025</v>
+        <v>1119</v>
       </c>
       <c r="CJ15" t="s">
-        <v>1026</v>
+        <v>1120</v>
       </c>
       <c r="CK15" t="s">
-        <v>1027</v>
+        <v>1121</v>
       </c>
       <c r="CL15" t="s">
-        <v>1028</v>
+        <v>1122</v>
       </c>
       <c r="CM15" t="s">
-        <v>1029</v>
+        <v>1123</v>
       </c>
       <c r="CN15" t="s">
-        <v>1030</v>
+        <v>1124</v>
       </c>
       <c r="CO15" t="s">
-        <v>1031</v>
+        <v>1125</v>
       </c>
       <c r="CP15" t="s">
-        <v>1032</v>
+        <v>1126</v>
       </c>
       <c r="CQ15" t="s">
-        <v>1033</v>
+        <v>1127</v>
       </c>
       <c r="CR15" t="s">
-        <v>1034</v>
+        <v>1128</v>
       </c>
       <c r="CS15" t="s">
+        <v>1129</v>
+      </c>
+      <c r="CT15" t="s">
+        <v>1130</v>
+      </c>
+      <c r="CU15" t="s">
+        <v>1131</v>
+      </c>
+      <c r="CV15" t="s">
+        <v>1132</v>
+      </c>
+      <c r="CW15" t="s">
+        <v>1133</v>
+      </c>
+      <c r="CX15" t="s">
+        <v>1134</v>
+      </c>
+      <c r="CY15" t="s">
+        <v>1135</v>
+      </c>
+      <c r="CZ15" t="s">
+        <v>1136</v>
+      </c>
+      <c r="DA15" t="s">
+        <v>1137</v>
+      </c>
+      <c r="DB15" t="s">
+        <v>1138</v>
+      </c>
+      <c r="DC15" t="s">
+        <v>1139</v>
+      </c>
+      <c r="DD15" t="s">
+        <v>1140</v>
+      </c>
+      <c r="DE15" t="s">
+        <v>1141</v>
+      </c>
+      <c r="DF15" t="s">
+        <v>1118</v>
+      </c>
+      <c r="DG15" t="s">
+        <v>1142</v>
+      </c>
+      <c r="DH15" t="s">
+        <v>1037</v>
+      </c>
+      <c r="DI15" t="s">
+        <v>1143</v>
+      </c>
+      <c r="DJ15" t="s">
+        <v>1144</v>
+      </c>
+      <c r="DK15" t="s">
+        <v>1145</v>
+      </c>
+      <c r="DL15" t="s">
+        <v>1146</v>
+      </c>
+      <c r="DM15" t="s">
+        <v>1147</v>
+      </c>
+      <c r="DN15" t="s">
+        <v>1148</v>
+      </c>
+      <c r="DO15" t="s">
+        <v>1149</v>
+      </c>
+      <c r="DP15" t="s">
+        <v>1150</v>
+      </c>
+      <c r="DQ15" t="s">
+        <v>1151</v>
+      </c>
+      <c r="DR15" t="s">
+        <v>1152</v>
+      </c>
+      <c r="DS15" t="s">
+        <v>1153</v>
+      </c>
+      <c r="DT15" t="s">
+        <v>1154</v>
+      </c>
+      <c r="DU15" t="s">
+        <v>1155</v>
+      </c>
+      <c r="DV15" t="s">
+        <v>1156</v>
+      </c>
+      <c r="DW15" t="s">
+        <v>1157</v>
+      </c>
+      <c r="DX15" t="s">
+        <v>1158</v>
+      </c>
+      <c r="DY15" t="s">
+        <v>1159</v>
+      </c>
+      <c r="DZ15" t="s">
+        <v>1160</v>
+      </c>
+      <c r="EA15" t="s">
+        <v>1161</v>
+      </c>
+      <c r="EB15" t="s">
+        <v>1162</v>
+      </c>
+      <c r="EC15" t="s">
+        <v>1163</v>
+      </c>
+      <c r="ED15" t="s">
+        <v>1164</v>
+      </c>
+      <c r="EE15" t="s">
+        <v>1165</v>
+      </c>
+      <c r="EF15" t="s">
+        <v>1126</v>
+      </c>
+      <c r="EG15" t="s">
+        <v>1166</v>
+      </c>
+      <c r="EH15" t="s">
+        <v>1167</v>
+      </c>
+      <c r="EI15" t="s">
+        <v>1168</v>
+      </c>
+      <c r="EJ15" t="s">
+        <v>1169</v>
+      </c>
+      <c r="EK15" t="s">
+        <v>1170</v>
+      </c>
+      <c r="EL15" t="s">
+        <v>1171</v>
+      </c>
+      <c r="EM15" t="s">
+        <v>1172</v>
+      </c>
+      <c r="EN15" t="s">
+        <v>1173</v>
+      </c>
+      <c r="EO15" t="s">
+        <v>1174</v>
+      </c>
+      <c r="EP15" t="s">
+        <v>1175</v>
+      </c>
+      <c r="EQ15" t="s">
+        <v>1176</v>
+      </c>
+      <c r="ER15" t="s">
+        <v>1177</v>
+      </c>
+      <c r="ES15" t="s">
+        <v>1178</v>
+      </c>
+      <c r="ET15" t="s">
+        <v>1179</v>
+      </c>
+      <c r="EU15" t="s">
         <v>1035</v>
       </c>
-      <c r="CT15" t="s">
-        <v>1036</v>
-      </c>
-      <c r="CU15" t="s">
-        <v>1037</v>
-      </c>
-      <c r="CV15" t="s">
-        <v>1038</v>
-      </c>
-      <c r="CW15" t="s">
-        <v>1039</v>
-      </c>
-      <c r="CX15" t="s">
-        <v>1040</v>
-      </c>
-      <c r="CY15" t="s">
-        <v>1041</v>
-      </c>
-      <c r="CZ15" t="s">
-        <v>1042</v>
-      </c>
-      <c r="DA15" t="s">
-        <v>1043</v>
-      </c>
-      <c r="DB15" t="s">
-        <v>1044</v>
-      </c>
-      <c r="DC15" t="s">
-        <v>1045</v>
-      </c>
-      <c r="DD15" t="s">
-        <v>1046</v>
-      </c>
-      <c r="DE15" t="s">
-        <v>1047</v>
-      </c>
-      <c r="DF15" t="s">
-        <v>1024</v>
-      </c>
-      <c r="DG15" t="s">
-        <v>1048</v>
-      </c>
-      <c r="DH15" t="s">
-        <v>943</v>
-      </c>
-      <c r="DI15" t="s">
-        <v>1049</v>
-      </c>
-      <c r="DJ15" t="s">
-        <v>1050</v>
-      </c>
-      <c r="DK15" t="s">
-        <v>1051</v>
-      </c>
-      <c r="DL15" t="s">
-        <v>1052</v>
-      </c>
-      <c r="DM15" t="s">
-        <v>1053</v>
-      </c>
-      <c r="DN15" t="s">
-        <v>1054</v>
-      </c>
-      <c r="DO15" t="s">
-        <v>1055</v>
-      </c>
-      <c r="DP15" t="s">
-        <v>1056</v>
-      </c>
-      <c r="DQ15" t="s">
-        <v>1057</v>
-      </c>
-      <c r="DR15" t="s">
-        <v>1058</v>
-      </c>
-      <c r="DS15" t="s">
-        <v>1059</v>
-      </c>
-      <c r="DT15" t="s">
-        <v>1060</v>
-      </c>
-      <c r="DU15" t="s">
-        <v>1061</v>
-      </c>
-      <c r="DV15" t="s">
-        <v>1062</v>
-      </c>
-      <c r="DW15" t="s">
-        <v>1063</v>
-      </c>
-      <c r="DX15" t="s">
-        <v>1064</v>
-      </c>
-      <c r="DY15" t="s">
-        <v>1065</v>
-      </c>
-      <c r="DZ15" t="s">
-        <v>1066</v>
-      </c>
-      <c r="EA15" t="s">
-        <v>1067</v>
-      </c>
-      <c r="EB15" t="s">
-        <v>1068</v>
-      </c>
-      <c r="EC15" t="s">
-        <v>1069</v>
-      </c>
-      <c r="ED15" t="s">
-        <v>1070</v>
-      </c>
-      <c r="EE15" t="s">
-        <v>1071</v>
-      </c>
-      <c r="EF15" t="s">
-        <v>1032</v>
-      </c>
-      <c r="EG15" t="s">
-        <v>1072</v>
-      </c>
-      <c r="EH15" t="s">
-        <v>1073</v>
-      </c>
-      <c r="EI15" t="s">
-        <v>1074</v>
-      </c>
-      <c r="EJ15" t="s">
-        <v>1075</v>
-      </c>
-      <c r="EK15" t="s">
-        <v>1076</v>
-      </c>
-      <c r="EL15" t="s">
-        <v>1077</v>
-      </c>
-      <c r="EM15" t="s">
-        <v>1078</v>
-      </c>
-      <c r="EN15" t="s">
-        <v>1079</v>
-      </c>
-      <c r="EO15" t="s">
-        <v>1080</v>
-      </c>
-      <c r="EP15" t="s">
-        <v>1081</v>
-      </c>
-      <c r="EQ15" t="s">
-        <v>1082</v>
-      </c>
-      <c r="ER15" t="s">
-        <v>1083</v>
-      </c>
-      <c r="ES15" t="s">
-        <v>1084</v>
-      </c>
-      <c r="ET15" t="s">
-        <v>1085</v>
-      </c>
-      <c r="EU15" t="s">
-        <v>941</v>
-      </c>
       <c r="EV15" t="s">
-        <v>1086</v>
+        <v>1180</v>
       </c>
       <c r="EW15" t="s">
-        <v>1087</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="16" spans="1:152">
       <c r="A16" t="s">
-        <v>1088</v>
+        <v>1182</v>
       </c>
       <c r="B16" t="s">
-        <v>1089</v>
+        <v>1183</v>
       </c>
       <c r="C16" t="s">
-        <v>1090</v>
+        <v>1184</v>
       </c>
       <c r="D16" t="s">
-        <v>1091</v>
+        <v>1185</v>
       </c>
       <c r="E16" t="s">
-        <v>1092</v>
+        <v>1186</v>
       </c>
       <c r="F16" t="s">
-        <v>1093</v>
+        <v>1187</v>
       </c>
       <c r="G16" t="s">
-        <v>1094</v>
+        <v>1188</v>
       </c>
       <c r="H16" t="s">
-        <v>1095</v>
+        <v>1189</v>
       </c>
       <c r="I16" t="s">
-        <v>1096</v>
+        <v>1190</v>
       </c>
       <c r="J16" t="s">
-        <v>1097</v>
+        <v>1191</v>
       </c>
       <c r="K16" t="s">
-        <v>1098</v>
+        <v>1192</v>
       </c>
       <c r="L16" t="s">
-        <v>1099</v>
+        <v>1193</v>
       </c>
       <c r="M16" t="s">
-        <v>1100</v>
+        <v>1194</v>
       </c>
       <c r="N16" t="s">
-        <v>1101</v>
+        <v>1195</v>
       </c>
       <c r="O16" t="s">
-        <v>1102</v>
+        <v>1196</v>
       </c>
       <c r="P16" t="s">
-        <v>1103</v>
+        <v>1197</v>
       </c>
       <c r="Q16" t="s">
-        <v>1104</v>
+        <v>1198</v>
       </c>
       <c r="R16" t="s">
-        <v>1105</v>
+        <v>1199</v>
       </c>
       <c r="S16" t="s">
-        <v>1106</v>
+        <v>1200</v>
       </c>
       <c r="T16" t="s">
-        <v>1107</v>
+        <v>1201</v>
       </c>
       <c r="U16" t="s">
-        <v>1108</v>
+        <v>1202</v>
       </c>
       <c r="V16" t="s">
-        <v>1109</v>
+        <v>1203</v>
       </c>
       <c r="W16" t="s">
-        <v>1110</v>
+        <v>1204</v>
       </c>
       <c r="X16" t="s">
-        <v>1111</v>
+        <v>1205</v>
       </c>
       <c r="Y16" t="s">
-        <v>1112</v>
+        <v>1206</v>
       </c>
       <c r="Z16" t="s">
-        <v>1113</v>
+        <v>1207</v>
       </c>
       <c r="AA16" t="s">
-        <v>1114</v>
+        <v>1208</v>
       </c>
       <c r="AB16" t="s">
-        <v>1115</v>
+        <v>1209</v>
       </c>
       <c r="AC16" t="s">
-        <v>1116</v>
+        <v>1210</v>
       </c>
       <c r="AD16" t="s">
-        <v>1117</v>
+        <v>1211</v>
       </c>
       <c r="AE16" t="s">
-        <v>1118</v>
+        <v>1212</v>
       </c>
       <c r="AF16" t="s">
-        <v>1119</v>
+        <v>1213</v>
       </c>
       <c r="AG16" t="s">
-        <v>1120</v>
+        <v>1214</v>
       </c>
       <c r="AH16" t="s">
-        <v>1121</v>
+        <v>1215</v>
       </c>
       <c r="AI16" t="s">
-        <v>1122</v>
+        <v>1216</v>
       </c>
       <c r="AJ16" t="s">
-        <v>1123</v>
+        <v>1217</v>
       </c>
       <c r="AK16" t="s">
-        <v>1124</v>
+        <v>1218</v>
       </c>
       <c r="AL16" t="s">
-        <v>1125</v>
+        <v>1219</v>
       </c>
       <c r="AM16" t="s">
-        <v>1126</v>
+        <v>1220</v>
       </c>
       <c r="AN16" t="s">
-        <v>1127</v>
+        <v>1221</v>
       </c>
       <c r="AO16" t="s">
-        <v>1128</v>
+        <v>1222</v>
       </c>
       <c r="AP16" t="s">
-        <v>1129</v>
+        <v>1223</v>
       </c>
       <c r="AQ16" t="s">
-        <v>1130</v>
+        <v>1224</v>
       </c>
       <c r="AR16" t="s">
-        <v>1131</v>
+        <v>1225</v>
       </c>
       <c r="AS16" t="s">
-        <v>1132</v>
+        <v>1226</v>
       </c>
       <c r="AT16" t="s">
-        <v>1133</v>
+        <v>1227</v>
       </c>
       <c r="AU16" t="s">
-        <v>1134</v>
+        <v>1228</v>
       </c>
       <c r="AV16" t="s">
-        <v>1135</v>
+        <v>1229</v>
       </c>
       <c r="AW16" t="s">
-        <v>1136</v>
+        <v>1230</v>
       </c>
       <c r="AX16" t="s">
-        <v>1137</v>
+        <v>1231</v>
       </c>
       <c r="AY16" t="s">
-        <v>1138</v>
+        <v>1232</v>
       </c>
       <c r="AZ16" t="s">
-        <v>1139</v>
+        <v>1233</v>
       </c>
       <c r="BA16" t="s">
-        <v>1140</v>
+        <v>1234</v>
       </c>
       <c r="BB16" t="s">
-        <v>1141</v>
+        <v>1235</v>
       </c>
       <c r="BC16" t="s">
-        <v>1142</v>
+        <v>1236</v>
       </c>
       <c r="BD16" t="s">
-        <v>1143</v>
+        <v>1237</v>
       </c>
       <c r="BE16" t="s">
-        <v>1144</v>
+        <v>1238</v>
       </c>
       <c r="BF16" t="s">
-        <v>1145</v>
+        <v>1239</v>
       </c>
       <c r="BG16" t="s">
-        <v>1146</v>
+        <v>1240</v>
       </c>
       <c r="BH16" t="s">
-        <v>1147</v>
+        <v>1241</v>
       </c>
       <c r="BI16" t="s">
-        <v>1148</v>
+        <v>1242</v>
       </c>
       <c r="BJ16" t="s">
-        <v>1149</v>
+        <v>1243</v>
       </c>
       <c r="BK16" t="s">
-        <v>1150</v>
+        <v>1244</v>
       </c>
       <c r="BL16" t="s">
-        <v>1151</v>
+        <v>1245</v>
       </c>
       <c r="BM16" t="s">
-        <v>1152</v>
+        <v>1246</v>
       </c>
       <c r="BN16" t="s">
-        <v>1153</v>
+        <v>1247</v>
       </c>
       <c r="BO16" t="s">
         <v>5</v>
       </c>
       <c r="BP16" t="s">
-        <v>1154</v>
+        <v>1248</v>
       </c>
       <c r="BQ16" t="s">
-        <v>1155</v>
+        <v>1249</v>
       </c>
       <c r="BR16" t="s">
-        <v>1156</v>
+        <v>1250</v>
       </c>
       <c r="BS16" t="s">
-        <v>1157</v>
+        <v>1251</v>
       </c>
       <c r="BT16" t="s">
-        <v>1158</v>
+        <v>1252</v>
       </c>
       <c r="BU16" t="s">
-        <v>1159</v>
+        <v>1253</v>
       </c>
       <c r="BV16" t="s">
-        <v>1160</v>
+        <v>1254</v>
       </c>
       <c r="BW16" t="s">
-        <v>1161</v>
+        <v>1255</v>
       </c>
       <c r="BX16" t="s">
-        <v>1162</v>
+        <v>1256</v>
       </c>
       <c r="BY16" t="s">
-        <v>1163</v>
+        <v>1257</v>
       </c>
       <c r="BZ16" t="s">
-        <v>1164</v>
+        <v>1258</v>
       </c>
       <c r="CA16" t="s">
-        <v>1165</v>
+        <v>1259</v>
       </c>
       <c r="CB16" t="s">
-        <v>1166</v>
+        <v>1260</v>
       </c>
       <c r="CC16" t="s">
-        <v>1167</v>
+        <v>1261</v>
       </c>
       <c r="CD16" t="s">
-        <v>1168</v>
+        <v>1262</v>
       </c>
       <c r="CE16" t="s">
-        <v>1169</v>
+        <v>1263</v>
       </c>
       <c r="CF16" t="s">
-        <v>1170</v>
+        <v>1264</v>
       </c>
       <c r="CG16" t="s">
-        <v>1171</v>
+        <v>1265</v>
       </c>
       <c r="CH16" t="s">
-        <v>1172</v>
+        <v>1266</v>
       </c>
       <c r="CI16" t="s">
-        <v>1173</v>
+        <v>1267</v>
       </c>
       <c r="CJ16" t="s">
-        <v>1174</v>
+        <v>1268</v>
       </c>
       <c r="CK16" t="s">
-        <v>1175</v>
+        <v>1269</v>
       </c>
       <c r="CL16" t="s">
-        <v>1176</v>
+        <v>1270</v>
       </c>
       <c r="CM16" t="s">
-        <v>1177</v>
+        <v>1271</v>
       </c>
       <c r="CN16" t="s">
-        <v>1178</v>
+        <v>1272</v>
       </c>
       <c r="CO16" t="s">
-        <v>1179</v>
+        <v>1273</v>
       </c>
       <c r="CP16" t="s">
-        <v>1180</v>
+        <v>1274</v>
       </c>
       <c r="CQ16" t="s">
-        <v>1181</v>
+        <v>1275</v>
       </c>
       <c r="CR16" t="s">
-        <v>1182</v>
+        <v>1276</v>
       </c>
       <c r="CS16" t="s">
-        <v>1183</v>
+        <v>1277</v>
       </c>
       <c r="CT16" t="s">
-        <v>1184</v>
+        <v>1278</v>
       </c>
       <c r="CU16" t="s">
-        <v>1185</v>
+        <v>1279</v>
       </c>
       <c r="CV16" t="s">
-        <v>1186</v>
+        <v>1280</v>
       </c>
       <c r="CW16" t="s">
-        <v>1187</v>
+        <v>1281</v>
       </c>
       <c r="CX16" t="s">
-        <v>1188</v>
+        <v>1282</v>
       </c>
       <c r="CY16" t="s">
-        <v>1189</v>
+        <v>1283</v>
       </c>
       <c r="CZ16" t="s">
-        <v>1190</v>
+        <v>1284</v>
       </c>
       <c r="DA16" t="s">
-        <v>1191</v>
+        <v>1285</v>
       </c>
       <c r="DB16" t="s">
-        <v>1192</v>
+        <v>1286</v>
       </c>
       <c r="DC16" t="s">
-        <v>1193</v>
+        <v>1287</v>
       </c>
       <c r="DD16" t="s">
-        <v>1194</v>
+        <v>1288</v>
       </c>
       <c r="DE16" t="s">
-        <v>1195</v>
+        <v>1289</v>
       </c>
       <c r="DF16" t="s">
-        <v>1196</v>
+        <v>1290</v>
       </c>
       <c r="DG16" t="s">
-        <v>1197</v>
+        <v>1291</v>
       </c>
       <c r="DH16" t="s">
-        <v>1198</v>
+        <v>1292</v>
       </c>
       <c r="DI16" t="s">
-        <v>1199</v>
+        <v>1293</v>
       </c>
       <c r="DJ16" t="s">
-        <v>1200</v>
+        <v>1294</v>
       </c>
       <c r="DK16" t="s">
-        <v>1201</v>
+        <v>1295</v>
       </c>
       <c r="DL16" t="s">
-        <v>1202</v>
+        <v>1296</v>
       </c>
       <c r="DM16" t="s">
-        <v>1203</v>
+        <v>1297</v>
       </c>
       <c r="DN16" t="s">
-        <v>1204</v>
+        <v>1298</v>
       </c>
       <c r="DO16" t="s">
-        <v>1205</v>
+        <v>1299</v>
       </c>
       <c r="DP16" t="s">
-        <v>1206</v>
+        <v>1300</v>
       </c>
       <c r="DQ16" t="s">
-        <v>1207</v>
+        <v>1301</v>
       </c>
       <c r="DR16" t="s">
-        <v>1208</v>
+        <v>1302</v>
       </c>
       <c r="DS16" t="s">
-        <v>1209</v>
+        <v>1303</v>
       </c>
       <c r="DT16" t="s">
-        <v>1210</v>
+        <v>1304</v>
       </c>
       <c r="DU16" t="s">
-        <v>1211</v>
+        <v>1305</v>
       </c>
       <c r="DV16" t="s">
-        <v>1212</v>
+        <v>1306</v>
       </c>
       <c r="DW16" t="s">
-        <v>1213</v>
+        <v>1307</v>
       </c>
       <c r="DX16" t="s">
-        <v>1214</v>
+        <v>1308</v>
       </c>
       <c r="DY16" t="s">
-        <v>1215</v>
+        <v>1309</v>
       </c>
       <c r="DZ16" t="s">
-        <v>1216</v>
+        <v>1310</v>
       </c>
       <c r="EA16" t="s">
-        <v>1217</v>
+        <v>1311</v>
       </c>
       <c r="EB16" t="s">
-        <v>1218</v>
+        <v>1312</v>
       </c>
       <c r="EC16" t="s">
-        <v>1219</v>
+        <v>1313</v>
       </c>
       <c r="ED16" t="s">
-        <v>1220</v>
+        <v>1314</v>
       </c>
       <c r="EE16" t="s">
-        <v>1221</v>
+        <v>1315</v>
       </c>
       <c r="EF16" t="s">
-        <v>1222</v>
+        <v>1316</v>
       </c>
       <c r="EG16" t="s">
-        <v>1223</v>
+        <v>1317</v>
       </c>
       <c r="EH16" t="s">
-        <v>1224</v>
+        <v>1318</v>
       </c>
       <c r="EI16" t="s">
-        <v>1225</v>
+        <v>1319</v>
       </c>
       <c r="EJ16" t="s">
-        <v>1226</v>
+        <v>1320</v>
       </c>
       <c r="EK16" t="s">
-        <v>1222</v>
+        <v>1316</v>
       </c>
       <c r="EL16" t="s">
-        <v>1227</v>
+        <v>1321</v>
       </c>
       <c r="EM16" t="s">
-        <v>1228</v>
+        <v>1322</v>
       </c>
       <c r="EN16" t="s">
-        <v>1229</v>
+        <v>1323</v>
       </c>
       <c r="EO16" t="s">
-        <v>1230</v>
+        <v>1324</v>
       </c>
       <c r="EP16" t="s">
-        <v>1231</v>
+        <v>1325</v>
       </c>
       <c r="EQ16" t="s">
-        <v>1232</v>
+        <v>1326</v>
       </c>
       <c r="ER16" t="s">
-        <v>1233</v>
+        <v>1327</v>
       </c>
       <c r="ES16" t="s">
-        <v>1234</v>
+        <v>1328</v>
       </c>
       <c r="ET16" t="s">
-        <v>1235</v>
+        <v>1329</v>
       </c>
       <c r="EU16" t="s">
-        <v>1236</v>
+        <v>1330</v>
       </c>
       <c r="EV16" t="s">
-        <v>1237</v>
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="17" spans="1:71">
+      <c r="A17" t="s">
+        <v>1332</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1335</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1336</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1337</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H17" t="s">
+        <v>1339</v>
+      </c>
+      <c r="I17" t="s">
+        <v>1340</v>
+      </c>
+      <c r="J17" t="s">
+        <v>1341</v>
+      </c>
+      <c r="K17" t="s">
+        <v>1342</v>
+      </c>
+      <c r="L17" t="s">
+        <v>1343</v>
+      </c>
+      <c r="M17" t="s">
+        <v>1344</v>
+      </c>
+      <c r="N17" t="s">
+        <v>1345</v>
+      </c>
+      <c r="O17" t="s">
+        <v>1346</v>
+      </c>
+      <c r="P17" t="s">
+        <v>1347</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>1348</v>
+      </c>
+      <c r="R17" t="s">
+        <v>272</v>
+      </c>
+      <c r="S17" t="s">
+        <v>1349</v>
+      </c>
+      <c r="T17" t="s">
+        <v>1350</v>
+      </c>
+      <c r="U17" t="s">
+        <v>1351</v>
+      </c>
+      <c r="V17" t="s">
+        <v>1352</v>
+      </c>
+      <c r="W17" t="s">
+        <v>403</v>
+      </c>
+      <c r="X17" t="s">
+        <v>692</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>1353</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>1354</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>1355</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>1356</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>1357</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>1358</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>1359</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>1360</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>1361</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>1362</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>1363</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>1364</v>
+      </c>
+      <c r="AK17" t="s">
+        <v>1365</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>1366</v>
+      </c>
+      <c r="AM17" t="s">
+        <v>1367</v>
+      </c>
+      <c r="AN17" t="s">
+        <v>1368</v>
+      </c>
+      <c r="AO17" t="s">
+        <v>1369</v>
+      </c>
+      <c r="AP17" t="s">
+        <v>1370</v>
+      </c>
+      <c r="AQ17" t="s">
+        <v>1371</v>
+      </c>
+      <c r="AR17" t="s">
+        <v>1372</v>
+      </c>
+      <c r="AS17" t="s">
+        <v>1373</v>
+      </c>
+      <c r="AT17" t="s">
+        <v>1374</v>
+      </c>
+      <c r="AU17" t="s">
+        <v>1375</v>
+      </c>
+      <c r="AV17" t="s">
+        <v>1376</v>
+      </c>
+      <c r="AW17" t="s">
+        <v>1377</v>
+      </c>
+      <c r="AX17" t="s">
+        <v>1378</v>
+      </c>
+      <c r="AY17" t="s">
+        <v>1379</v>
+      </c>
+      <c r="AZ17" t="s">
+        <v>1380</v>
+      </c>
+      <c r="BA17" t="s">
+        <v>1381</v>
+      </c>
+      <c r="BB17" t="s">
+        <v>1382</v>
+      </c>
+      <c r="BC17" t="s">
+        <v>1383</v>
+      </c>
+      <c r="BD17" t="s">
+        <v>1384</v>
+      </c>
+      <c r="BE17" t="s">
+        <v>1385</v>
+      </c>
+      <c r="BF17" t="s">
+        <v>1386</v>
+      </c>
+      <c r="BG17" t="s">
+        <v>1387</v>
+      </c>
+      <c r="BH17" t="s">
+        <v>1388</v>
+      </c>
+      <c r="BI17" t="s">
+        <v>1389</v>
+      </c>
+      <c r="BJ17" t="s">
+        <v>1390</v>
+      </c>
+      <c r="BK17" t="s">
+        <v>1391</v>
+      </c>
+      <c r="BL17" t="s">
+        <v>1392</v>
+      </c>
+      <c r="BM17" t="s">
+        <v>1393</v>
+      </c>
+      <c r="BN17" t="s">
+        <v>1394</v>
+      </c>
+      <c r="BO17" t="s">
+        <v>1395</v>
+      </c>
+      <c r="BP17" t="s">
+        <v>1396</v>
+      </c>
+      <c r="BQ17" t="s">
+        <v>1397</v>
+      </c>
+      <c r="BR17" t="s">
+        <v>1398</v>
+      </c>
+      <c r="BS17" t="s">
+        <v>1399</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="$A10:$XFD10">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="$A17:$XFD17">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="EP13:XFD13;A13:EN13">
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>

</xml_diff>